<commit_message>
- jira base uri is without any path
</commit_message>
<xml_diff>
--- a/zephyr-uploader/demo_zephyr.xlsx
+++ b/zephyr-uploader/demo_zephyr.xlsx
@@ -287,7 +287,7 @@
         <family val="3"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">http://jira.yourcompany.com/rest/
+      <t xml:space="preserve">http://jira.yourcompany.com
 </t>
     </r>
     <r>
@@ -1437,7 +1437,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1496,6 +1496,9 @@
   <mergeCells count="1">
     <mergeCell ref="D3:D5"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="http://jira.yourcompany.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>